<commit_message>
Moved to 100 kBit. Added DEBUG_TRANSMITTER define. Successfully adjusts address & timer.
</commit_message>
<xml_diff>
--- a/Foxlocket/FoxLocket.xlsx
+++ b/Foxlocket/FoxLocket.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>Timings</t>
   </si>
@@ -47,6 +47,18 @@
   </si>
   <si>
     <t>tics</t>
+  </si>
+  <si>
+    <t>Packet duration</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>WhenTransmit</t>
+  </si>
+  <si>
+    <t>To ease multiplication</t>
   </si>
 </sst>
 </file>
@@ -171,12 +183,13 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent1" xfId="4" builtinId="29"/>
@@ -482,23 +495,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:C8"/>
+  <dimension ref="A3:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="43.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -509,7 +523,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -517,7 +531,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -529,7 +543,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -540,7 +554,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -549,6 +563,64 @@
         <v>488.28125</v>
       </c>
       <c r="C8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>64</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3">
+        <f>B12*B11</f>
+        <v>640</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <f>B13/B6</f>
+        <v>625</v>
+      </c>
+      <c r="C14" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Working, timer divider = 1024
</commit_message>
<xml_diff>
--- a/Foxlocket/FoxLocket.xlsx
+++ b/Foxlocket/FoxLocket.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9114"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="19080" windowHeight="8475"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,9 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="Addr">Sheet1!$B$16</definedName>
     <definedName name="Fclk">Sheet1!$B$4</definedName>
+    <definedName name="Multi">Sheet1!$B$17</definedName>
     <definedName name="Tclk">Sheet1!#REF!</definedName>
   </definedNames>
   <calcPr calcId="144315"/>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>Timings</t>
   </si>
@@ -58,7 +60,40 @@
     <t>WhenTransmit</t>
   </si>
   <si>
-    <t>To ease multiplication</t>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Multiplier</t>
+  </si>
+  <si>
+    <t>Addr 1</t>
+  </si>
+  <si>
+    <t>Addr 2</t>
+  </si>
+  <si>
+    <t>Addr 3</t>
+  </si>
+  <si>
+    <t>Addr 4</t>
+  </si>
+  <si>
+    <t>Addr 5</t>
+  </si>
+  <si>
+    <t>Addr 6</t>
+  </si>
+  <si>
+    <t>Addr 7</t>
+  </si>
+  <si>
+    <t>Addr 8</t>
+  </si>
+  <si>
+    <t>Addr 9</t>
+  </si>
+  <si>
+    <t>Addr 10</t>
   </si>
 </sst>
 </file>
@@ -495,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D14"/>
+  <dimension ref="A3:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,12 +542,12 @@
     <col min="4" max="4" width="43.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -523,109 +558,259 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="4">
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3">
         <f>B5*1000/Fclk</f>
-        <v>1.024</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="4">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="3">
         <f>B7/B6</f>
-        <v>488.28125</v>
+        <v>3125</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="5">
-        <v>36</v>
+        <v>8.4</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B11">
-        <v>64</v>
+      <c r="B11" s="3">
+        <f>B10/B6</f>
+        <v>131.25</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
       </c>
-      <c r="D11" t="s">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="4">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="3">
+        <f>Addr*B17+B11</f>
+        <v>259.25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19">
+        <f>B18*B6</f>
+        <v>16.591999999999999</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="B21" s="4">
+        <v>7.4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="3">
+        <f>B21/B6</f>
+        <v>115.625</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <f>B25*Multi</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <f>B26*Multi</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <f>B27*Multi</f>
+        <v>384</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28">
+        <f>B28*Multi</f>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <f>B29*Multi</f>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30">
+        <v>6</v>
+      </c>
+      <c r="C30">
+        <f>B30*Multi</f>
+        <v>768</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31">
+        <v>7</v>
+      </c>
+      <c r="C31">
+        <f>B31*Multi</f>
+        <v>896</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32">
+        <v>8</v>
+      </c>
+      <c r="C32">
+        <f>B32*Multi</f>
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33">
+        <v>9</v>
+      </c>
+      <c r="C33">
+        <f>B33*Multi</f>
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34">
         <v>10</v>
       </c>
-      <c r="B12" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="3">
-        <f>B12*B11</f>
-        <v>640</v>
-      </c>
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14">
-        <f>B13/B6</f>
-        <v>625</v>
-      </c>
-      <c r="C14" t="s">
-        <v>8</v>
+      <c r="C34">
+        <f>B34*Multi</f>
+        <v>1280</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Working again. Timer1 divider = 64.
</commit_message>
<xml_diff>
--- a/Foxlocket/FoxLocket.xlsx
+++ b/Foxlocket/FoxLocket.xlsx
@@ -12,17 +12,19 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="Addr">Sheet1!$B$16</definedName>
+    <definedName name="Addr">Sheet1!#REF!</definedName>
     <definedName name="Fclk">Sheet1!$B$4</definedName>
-    <definedName name="Multi">Sheet1!$B$17</definedName>
+    <definedName name="Multi">Sheet1!$B$16</definedName>
     <definedName name="Tclk">Sheet1!#REF!</definedName>
+    <definedName name="tic_lng">Sheet1!$B$6</definedName>
+    <definedName name="tic_lngth">Sheet1!$B$6</definedName>
   </definedNames>
   <calcPr calcId="144315"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>Timings</t>
   </si>
@@ -51,49 +53,19 @@
     <t>tics</t>
   </si>
   <si>
-    <t>Packet duration</t>
-  </si>
-  <si>
     <t>Address</t>
   </si>
   <si>
-    <t>WhenTransmit</t>
-  </si>
-  <si>
     <t>Time</t>
   </si>
   <si>
     <t>Multiplier</t>
   </si>
   <si>
-    <t>Addr 1</t>
-  </si>
-  <si>
-    <t>Addr 2</t>
-  </si>
-  <si>
-    <t>Addr 3</t>
-  </si>
-  <si>
-    <t>Addr 4</t>
-  </si>
-  <si>
-    <t>Addr 5</t>
-  </si>
-  <si>
-    <t>Addr 6</t>
-  </si>
-  <si>
-    <t>Addr 7</t>
-  </si>
-  <si>
-    <t>Addr 8</t>
-  </si>
-  <si>
-    <t>Addr 9</t>
-  </si>
-  <si>
-    <t>Addr 10</t>
+    <t>IRQ to end of packet receiving</t>
+  </si>
+  <si>
+    <t>Experimental</t>
   </si>
 </sst>
 </file>
@@ -172,7 +144,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -210,6 +182,86 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -218,13 +270,27 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent1" xfId="4" builtinId="29"/>
@@ -530,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:C34"/>
+  <dimension ref="A3:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,12 +608,12 @@
     <col min="4" max="4" width="43.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -558,15 +624,24 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="4">
         <v>64</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -577,8 +652,19 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F6" s="8">
+        <v>1</v>
+      </c>
+      <c r="G6" s="9">
+        <f>F6*Multi</f>
+        <v>256</v>
+      </c>
+      <c r="H6" s="10">
+        <f>G6*tic_lng</f>
+        <v>16.384</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -588,8 +674,19 @@
       <c r="C7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F7" s="8">
+        <v>2</v>
+      </c>
+      <c r="G7" s="9">
+        <f>F7*Multi</f>
+        <v>512</v>
+      </c>
+      <c r="H7" s="10">
+        <f>G7*tic_lng</f>
+        <v>32.768000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -600,212 +697,156 @@
       <c r="C8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="F8" s="8">
+        <v>3</v>
+      </c>
+      <c r="G8" s="9">
+        <f>F8*Multi</f>
+        <v>768</v>
+      </c>
+      <c r="H8" s="10">
+        <f>G8*tic_lng</f>
+        <v>49.152000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F9" s="8">
+        <v>4</v>
+      </c>
+      <c r="G9" s="9">
+        <f>F9*Multi</f>
+        <v>1024</v>
+      </c>
+      <c r="H9" s="10">
+        <f>G9*tic_lng</f>
+        <v>65.536000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F10" s="8">
+        <v>5</v>
+      </c>
+      <c r="G10" s="9">
+        <f>F10*Multi</f>
+        <v>1280</v>
+      </c>
+      <c r="H10" s="10">
+        <f>G10*tic_lng</f>
+        <v>81.92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4">
+        <v>7.4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="8">
+        <v>6</v>
+      </c>
+      <c r="G11" s="9">
+        <f>F11*Multi</f>
+        <v>1536</v>
+      </c>
+      <c r="H11" s="10">
+        <f>G11*tic_lng</f>
+        <v>98.304000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3">
+        <f>B11/B6</f>
+        <v>115.625</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="8">
+        <v>7</v>
+      </c>
+      <c r="G12" s="9">
+        <f>F12*Multi</f>
+        <v>1792</v>
+      </c>
+      <c r="H12" s="10">
+        <f>G12*tic_lng</f>
+        <v>114.688</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="8">
+        <v>8</v>
+      </c>
+      <c r="G13" s="9">
+        <f>F13*Multi</f>
+        <v>2048</v>
+      </c>
+      <c r="H13" s="10">
+        <f>G13*tic_lng</f>
+        <v>131.072</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2">
+        <v>8.4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="8">
         <v>9</v>
       </c>
-      <c r="B10" s="5">
-        <v>8.4</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="3">
-        <f>B10/B6</f>
+      <c r="G14" s="9">
+        <f>F14*Multi</f>
+        <v>2304</v>
+      </c>
+      <c r="H14" s="10">
+        <f>G14*tic_lng</f>
+        <v>147.45600000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="3">
+        <f>B14/B6</f>
         <v>131.25</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C15" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F15" s="11">
+        <v>10</v>
+      </c>
+      <c r="G15" s="12">
+        <f>F15*Multi</f>
+        <v>2560</v>
+      </c>
+      <c r="H15" s="13">
+        <f>G15*tic_lng</f>
+        <v>163.84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="4">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="3">
-        <f>Addr*B17+B11</f>
-        <v>259.25</v>
-      </c>
-      <c r="C18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19">
-        <f>B18*B6</f>
-        <v>16.591999999999999</v>
-      </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="4">
-        <v>7.4</v>
-      </c>
-      <c r="C21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="3">
-        <f>B21/B6</f>
-        <v>115.625</v>
-      </c>
-      <c r="C22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25">
-        <f>B25*Multi</f>
-        <v>128</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26">
-        <v>2</v>
-      </c>
-      <c r="C26">
-        <f>B26*Multi</f>
+      <c r="B16">
         <v>256</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>16</v>
-      </c>
-      <c r="B27">
-        <v>3</v>
-      </c>
-      <c r="C27">
-        <f>B27*Multi</f>
-        <v>384</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28">
-        <v>4</v>
-      </c>
-      <c r="C28">
-        <f>B28*Multi</f>
-        <v>512</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>18</v>
-      </c>
-      <c r="B29">
-        <v>5</v>
-      </c>
-      <c r="C29">
-        <f>B29*Multi</f>
-        <v>640</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>19</v>
-      </c>
-      <c r="B30">
-        <v>6</v>
-      </c>
-      <c r="C30">
-        <f>B30*Multi</f>
-        <v>768</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>20</v>
-      </c>
-      <c r="B31">
-        <v>7</v>
-      </c>
-      <c r="C31">
-        <f>B31*Multi</f>
-        <v>896</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>21</v>
-      </c>
-      <c r="B32">
-        <v>8</v>
-      </c>
-      <c r="C32">
-        <f>B32*Multi</f>
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33">
-        <v>9</v>
-      </c>
-      <c r="C33">
-        <f>B33*Multi</f>
-        <v>1152</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34">
-        <v>10</v>
-      </c>
-      <c r="C34">
-        <f>B34*Multi</f>
-        <v>1280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Strange reaction, not always shows existance.
</commit_message>
<xml_diff>
--- a/Foxlocket/FoxLocket.xlsx
+++ b/Foxlocket/FoxLocket.xlsx
@@ -13,6 +13,7 @@
   </sheets>
   <definedNames>
     <definedName name="Addr">Sheet1!#REF!</definedName>
+    <definedName name="Fc">Sheet1!$B$25</definedName>
     <definedName name="Fclk">Sheet1!$B$4</definedName>
     <definedName name="Multi">Sheet1!$B$16</definedName>
     <definedName name="Tclk">Sheet1!#REF!</definedName>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>Timings</t>
   </si>
@@ -66,6 +67,24 @@
   </si>
   <si>
     <t>Experimental</t>
+  </si>
+  <si>
+    <t>Antenna calculations</t>
+  </si>
+  <si>
+    <t>Fcarrier</t>
+  </si>
+  <si>
+    <t>MHz</t>
+  </si>
+  <si>
+    <t>Wave length</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>WL/4</t>
   </si>
 </sst>
 </file>
@@ -270,7 +289,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3"/>
@@ -291,6 +310,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent1" xfId="4" builtinId="29"/>
@@ -596,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H16"/>
+  <dimension ref="A3:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,11 +676,11 @@
         <v>1</v>
       </c>
       <c r="G6" s="9">
-        <f>F6*Multi</f>
+        <f t="shared" ref="G6:G15" si="0">F6*Multi</f>
         <v>256</v>
       </c>
       <c r="H6" s="10">
-        <f>G6*tic_lng</f>
+        <f t="shared" ref="H6:H15" si="1">G6*tic_lng</f>
         <v>16.384</v>
       </c>
     </row>
@@ -678,11 +698,11 @@
         <v>2</v>
       </c>
       <c r="G7" s="9">
-        <f>F7*Multi</f>
+        <f t="shared" si="0"/>
         <v>512</v>
       </c>
       <c r="H7" s="10">
-        <f>G7*tic_lng</f>
+        <f t="shared" si="1"/>
         <v>32.768000000000001</v>
       </c>
     </row>
@@ -701,11 +721,11 @@
         <v>3</v>
       </c>
       <c r="G8" s="9">
-        <f>F8*Multi</f>
+        <f t="shared" si="0"/>
         <v>768</v>
       </c>
       <c r="H8" s="10">
-        <f>G8*tic_lng</f>
+        <f t="shared" si="1"/>
         <v>49.152000000000001</v>
       </c>
     </row>
@@ -714,11 +734,11 @@
         <v>4</v>
       </c>
       <c r="G9" s="9">
-        <f>F9*Multi</f>
+        <f t="shared" si="0"/>
         <v>1024</v>
       </c>
       <c r="H9" s="10">
-        <f>G9*tic_lng</f>
+        <f t="shared" si="1"/>
         <v>65.536000000000001</v>
       </c>
     </row>
@@ -727,11 +747,11 @@
         <v>5</v>
       </c>
       <c r="G10" s="9">
-        <f>F10*Multi</f>
+        <f t="shared" si="0"/>
         <v>1280</v>
       </c>
       <c r="H10" s="10">
-        <f>G10*tic_lng</f>
+        <f t="shared" si="1"/>
         <v>81.92</v>
       </c>
     </row>
@@ -749,11 +769,11 @@
         <v>6</v>
       </c>
       <c r="G11" s="9">
-        <f>F11*Multi</f>
+        <f t="shared" si="0"/>
         <v>1536</v>
       </c>
       <c r="H11" s="10">
-        <f>G11*tic_lng</f>
+        <f t="shared" si="1"/>
         <v>98.304000000000002</v>
       </c>
     </row>
@@ -772,11 +792,11 @@
         <v>7</v>
       </c>
       <c r="G12" s="9">
-        <f>F12*Multi</f>
+        <f t="shared" si="0"/>
         <v>1792</v>
       </c>
       <c r="H12" s="10">
-        <f>G12*tic_lng</f>
+        <f t="shared" si="1"/>
         <v>114.688</v>
       </c>
     </row>
@@ -785,11 +805,11 @@
         <v>8</v>
       </c>
       <c r="G13" s="9">
-        <f>F13*Multi</f>
+        <f t="shared" si="0"/>
         <v>2048</v>
       </c>
       <c r="H13" s="10">
-        <f>G13*tic_lng</f>
+        <f t="shared" si="1"/>
         <v>131.072</v>
       </c>
     </row>
@@ -810,11 +830,11 @@
         <v>9</v>
       </c>
       <c r="G14" s="9">
-        <f>F14*Multi</f>
+        <f t="shared" si="0"/>
         <v>2304</v>
       </c>
       <c r="H14" s="10">
-        <f>G14*tic_lng</f>
+        <f t="shared" si="1"/>
         <v>147.45600000000002</v>
       </c>
     </row>
@@ -833,11 +853,11 @@
         <v>10</v>
       </c>
       <c r="G15" s="12">
-        <f>F15*Multi</f>
+        <f t="shared" si="0"/>
         <v>2560</v>
       </c>
       <c r="H15" s="13">
-        <f>G15*tic_lng</f>
+        <f t="shared" si="1"/>
         <v>163.84</v>
       </c>
     </row>
@@ -847,6 +867,46 @@
       </c>
       <c r="B16">
         <v>256</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25">
+        <v>315</v>
+      </c>
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="14">
+        <f>3*10^8/(Fc*10^6)</f>
+        <v>0.95238095238095233</v>
+      </c>
+      <c r="C26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="14">
+        <f>B26/4</f>
+        <v>0.23809523809523808</v>
+      </c>
+      <c r="C27" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>